<commit_message>
Data import and BC files
</commit_message>
<xml_diff>
--- a/scripts/datatools/IC/IC_From_DATA/Defaults_20191101.xlsx
+++ b/scripts/datatools/IC/IC_From_DATA/Defaults_20191101.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\datatools\IC\IC_From_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9723307E-B0A9-4B05-9D62-1A5214B43440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7BDC74-7EA1-48D7-8D0D-9D35507EB338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2430" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="2775" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults_20130301" sheetId="1" r:id="rId1"/>
@@ -994,7 +994,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,10 +1190,10 @@
       </c>
       <c r="H5">
         <f>(G5+I5)/2</f>
-        <v>34.735749999999996</v>
+        <v>52</v>
       </c>
       <c r="I5">
-        <v>45.471499999999999</v>
+        <v>80</v>
       </c>
       <c r="J5">
         <v>90</v>

</xml_diff>